<commit_message>
updated account statement for user by date
</commit_message>
<xml_diff>
--- a/src/uploads/1676981840300-40101888-Untitled spreadsheet (1).xlsx
+++ b/src/uploads/1676981840300-40101888-Untitled spreadsheet (1).xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="43">
   <si>
     <t>customerName</t>
   </si>
@@ -30,6 +30,12 @@
     <t>accountName</t>
   </si>
   <si>
+    <t>banktype</t>
+  </si>
+  <si>
+    <t>AccountType</t>
+  </si>
+  <si>
     <t>Folashade</t>
   </si>
   <si>
@@ -37,6 +43,12 @@
   </si>
   <si>
     <t>Demi John</t>
+  </si>
+  <si>
+    <t>Inter-bank</t>
+  </si>
+  <si>
+    <t>Savings</t>
   </si>
   <si>
     <t>Ade Tomas</t>
@@ -54,10 +66,16 @@
     <t>GT Bank</t>
   </si>
   <si>
+    <t>Intra-bank</t>
+  </si>
+  <si>
     <t>ade Tomas</t>
   </si>
   <si>
     <t>Chase Bank</t>
+  </si>
+  <si>
+    <t>Current</t>
   </si>
   <si>
     <t>Shina pellas</t>
@@ -130,12 +148,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <color theme="1"/>
@@ -161,10 +183,10 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -393,7 +415,7 @@
     <col customWidth="1" min="3" max="3" width="10.43"/>
     <col customWidth="1" min="4" max="4" width="14.86"/>
     <col customWidth="1" min="5" max="5" width="18.14"/>
-    <col customWidth="1" min="6" max="26" width="8.71"/>
+    <col customWidth="1" min="6" max="6" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -412,107 +434,149 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1">
         <v>20000.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1">
         <v>1.122364472E9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1">
         <v>50000.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1">
         <v>6.477364527E9</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>10</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1">
         <v>100000.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1">
         <v>2.837465539E9</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1">
         <v>60000.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1">
         <v>9.877364536E9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1">
         <v>90000.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1">
         <v>2.837453726E9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1">
         <v>150000.0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D7" s="1">
         <v>3.768267733E9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1"/>
@@ -1495,6 +1559,19 @@
     <row r="985" ht="15.75" customHeight="1"/>
     <row r="986" ht="15.75" customHeight="1"/>
     <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -1513,322 +1590,322 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="8.71"/>
+    <col customWidth="1" min="1" max="6" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>21</v>
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>10.0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>1.0</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="C2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <f t="shared" ref="A3:A20" si="1">(A2+10)</f>
         <v>20</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <f t="shared" ref="B3:B20" si="2">(B2+1)</f>
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="2">
+      <c r="C8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="2">
+      <c r="C9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="C10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="2">
+      <c r="C11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="2">
+      <c r="C12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="2">
+      <c r="C13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <f t="shared" si="1"/>
         <v>130</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="2">
+      <c r="C14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="2">
+      <c r="C15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <f t="shared" si="1"/>
         <v>150</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="2">
+      <c r="C16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <f t="shared" si="1"/>
         <v>160</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="2">
+      <c r="C17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <f t="shared" si="1"/>
         <v>170</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="2">
+      <c r="C18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <f t="shared" si="1"/>
         <v>180</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="2">
+      <c r="C19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <f t="shared" si="1"/>
         <v>190</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="2">
+      <c r="C20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="1">
         <v>500.0</v>
       </c>
     </row>
@@ -2830,322 +2907,322 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="8.71"/>
+    <col customWidth="1" min="1" max="6" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>21</v>
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>10.0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>1.0</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="C2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <f t="shared" ref="A3:A20" si="1">(A2+10)</f>
         <v>20</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <f t="shared" ref="B3:B20" si="2">(B2+1)</f>
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="2">
+      <c r="C8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="2">
+      <c r="C9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="C10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="2">
+      <c r="C11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="2">
+      <c r="C12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="2">
+      <c r="C13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <f t="shared" si="1"/>
         <v>130</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="2">
+      <c r="C14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="2">
+      <c r="C15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <f t="shared" si="1"/>
         <v>150</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="2">
+      <c r="C16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <f t="shared" si="1"/>
         <v>160</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="2">
+      <c r="C17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <f t="shared" si="1"/>
         <v>170</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="2">
+      <c r="C18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <f t="shared" si="1"/>
         <v>180</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="2">
+      <c r="C19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="1">
         <v>500.0</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <f t="shared" si="1"/>
         <v>190</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="2">
+      <c r="C20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="1">
         <v>500.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update on mail template
</commit_message>
<xml_diff>
--- a/src/uploads/1676981840300-40101888-Untitled spreadsheet (1).xlsx
+++ b/src/uploads/1676981840300-40101888-Untitled spreadsheet (1).xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="46">
   <si>
     <t>customerName</t>
   </si>
@@ -33,52 +33,61 @@
     <t>banktype</t>
   </si>
   <si>
-    <t>AccountType</t>
+    <t>accountType</t>
+  </si>
+  <si>
+    <t>bankCode</t>
   </si>
   <si>
     <t>Folashade</t>
   </si>
   <si>
+    <t>Stanbic IBTC Bank</t>
+  </si>
+  <si>
+    <t>0034551560</t>
+  </si>
+  <si>
+    <t>Prince Emmanuel Odu</t>
+  </si>
+  <si>
+    <t>Inter-bank</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
+    <t>Ade Tomas</t>
+  </si>
+  <si>
+    <t>Access Bank</t>
+  </si>
+  <si>
+    <t>SOLA tom</t>
+  </si>
+  <si>
+    <t>shayo martins</t>
+  </si>
+  <si>
+    <t>GT Bank</t>
+  </si>
+  <si>
+    <t>Intra-bank</t>
+  </si>
+  <si>
+    <t>ade Tomas</t>
+  </si>
+  <si>
+    <t>Chase Bank</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>Shina pellas</t>
+  </si>
+  <si>
     <t>First Bank</t>
-  </si>
-  <si>
-    <t>Demi John</t>
-  </si>
-  <si>
-    <t>Inter-bank</t>
-  </si>
-  <si>
-    <t>Savings</t>
-  </si>
-  <si>
-    <t>Ade Tomas</t>
-  </si>
-  <si>
-    <t>Access Bank</t>
-  </si>
-  <si>
-    <t>SOLA tom</t>
-  </si>
-  <si>
-    <t>shayo martins</t>
-  </si>
-  <si>
-    <t>GT Bank</t>
-  </si>
-  <si>
-    <t>Intra-bank</t>
-  </si>
-  <si>
-    <t>ade Tomas</t>
-  </si>
-  <si>
-    <t>Chase Bank</t>
-  </si>
-  <si>
-    <t>Current</t>
-  </si>
-  <si>
-    <t>Shina pellas</t>
   </si>
   <si>
     <t>Ayomide Thompson</t>
@@ -179,12 +188,18 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -440,143 +455,164 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1">
         <v>20000.0</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1.122364472E9</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="H2" s="2">
+        <v>221.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1">
         <v>50000.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1">
         <v>6.477364527E9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="H3" s="2">
+        <v>21.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1">
         <v>100000.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1">
         <v>2.837465539E9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="H4" s="2">
+        <v>200.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1">
         <v>60000.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D5" s="1">
         <v>9.877364536E9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="H5" s="2">
+        <v>341.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1">
         <v>90000.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1">
         <v>2.837453726E9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="H6" s="2">
+        <v>245.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1">
         <v>150000.0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1">
         <v>3.768267733E9</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>20</v>
+      <c r="H7" s="2">
+        <v>200.0</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1"/>
@@ -1595,16 +1631,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2">
@@ -1615,7 +1651,7 @@
         <v>1.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D2" s="1">
         <v>500.0</v>
@@ -1631,7 +1667,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1">
         <v>500.0</v>
@@ -1647,7 +1683,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D4" s="1">
         <v>500.0</v>
@@ -1663,7 +1699,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D5" s="1">
         <v>500.0</v>
@@ -1679,7 +1715,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D6" s="1">
         <v>500.0</v>
@@ -1695,7 +1731,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D7" s="1">
         <v>500.0</v>
@@ -1711,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D8" s="1">
         <v>500.0</v>
@@ -1727,7 +1763,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D9" s="1">
         <v>500.0</v>
@@ -1743,7 +1779,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D10" s="1">
         <v>500.0</v>
@@ -1759,7 +1795,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D11" s="1">
         <v>500.0</v>
@@ -1775,7 +1811,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D12" s="1">
         <v>500.0</v>
@@ -1791,7 +1827,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1">
         <v>500.0</v>
@@ -1807,7 +1843,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D14" s="1">
         <v>500.0</v>
@@ -1823,7 +1859,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D15" s="1">
         <v>500.0</v>
@@ -1839,7 +1875,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D16" s="1">
         <v>500.0</v>
@@ -1855,7 +1891,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D17" s="1">
         <v>500.0</v>
@@ -1871,7 +1907,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D18" s="1">
         <v>500.0</v>
@@ -1887,7 +1923,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D19" s="1">
         <v>500.0</v>
@@ -1903,7 +1939,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D20" s="1">
         <v>500.0</v>
@@ -2912,16 +2948,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2">
@@ -2932,7 +2968,7 @@
         <v>1.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D2" s="1">
         <v>500.0</v>
@@ -2948,7 +2984,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1">
         <v>500.0</v>
@@ -2964,7 +3000,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D4" s="1">
         <v>500.0</v>
@@ -2980,7 +3016,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D5" s="1">
         <v>500.0</v>
@@ -2996,7 +3032,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D6" s="1">
         <v>500.0</v>
@@ -3012,7 +3048,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D7" s="1">
         <v>500.0</v>
@@ -3028,7 +3064,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D8" s="1">
         <v>500.0</v>
@@ -3044,7 +3080,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D9" s="1">
         <v>500.0</v>
@@ -3060,7 +3096,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D10" s="1">
         <v>500.0</v>
@@ -3076,7 +3112,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D11" s="1">
         <v>500.0</v>
@@ -3092,7 +3128,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D12" s="1">
         <v>500.0</v>
@@ -3108,7 +3144,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1">
         <v>500.0</v>
@@ -3124,7 +3160,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D14" s="1">
         <v>500.0</v>
@@ -3140,7 +3176,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D15" s="1">
         <v>500.0</v>
@@ -3156,7 +3192,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D16" s="1">
         <v>500.0</v>
@@ -3172,7 +3208,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D17" s="1">
         <v>500.0</v>
@@ -3188,7 +3224,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D18" s="1">
         <v>500.0</v>
@@ -3204,7 +3240,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D19" s="1">
         <v>500.0</v>
@@ -3220,7 +3256,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D20" s="1">
         <v>500.0</v>

</xml_diff>